<commit_message>
PosterPresentationFINAL is pushed and extra drafts removed.
</commit_message>
<xml_diff>
--- a/ANDY Use These Files/Jodi Unique Corpus/Top50Words_Tabbed.xlsx
+++ b/ANDY Use These Files/Jodi Unique Corpus/Top50Words_Tabbed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jodip\Documents\GitHub\Capstone\ANDY Use These Files\Jodi Unique Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1C2156-7042-46B1-8275-1C525461C20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D8007-3D7B-4373-BAAB-E76864160575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" firstSheet="4" activeTab="8" xr2:uid="{7D602C9B-6754-46D4-A825-AD2B7971C5CF}"/>
+    <workbookView xWindow="-10188" yWindow="2472" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="8" xr2:uid="{7D602C9B-6754-46D4-A825-AD2B7971C5CF}"/>
   </bookViews>
   <sheets>
     <sheet name="DataScientistCount" sheetId="5" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Sheet2" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataScientistCount!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$J$1:$J$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sheet4!$A$1:$H$133</definedName>
   </definedNames>
@@ -634,7 +635,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +702,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -732,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -766,7 +779,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -780,10 +792,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3713,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC81E68B-CB25-4682-BD0B-005BF9576A2F}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C51"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3732,555 +3757,560 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>171</v>
       </c>
       <c r="C2">
-        <v>638</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="C3">
-        <v>497</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C4">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <v>420</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>367</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>362</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8">
-        <v>361</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C9">
-        <v>346</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>339</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>320</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>306</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>301</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C14">
-        <v>299</v>
+        <v>638</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="C15">
-        <v>293</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C16">
-        <v>274</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>268</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>252</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C20">
-        <v>236</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>235</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C22">
-        <v>225</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="C23">
-        <v>222</v>
+        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C24">
-        <v>220</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="C25">
-        <v>217</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>169</v>
       </c>
       <c r="C26">
-        <v>216</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="C27">
-        <v>213</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="C28">
-        <v>208</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C29">
-        <v>202</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="C30">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="C31">
-        <v>198</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C32">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C33">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>185</v>
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="C35">
-        <v>177</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>177</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C38">
-        <v>170</v>
+        <v>497</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="C39">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C40">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C41">
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>165</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>16</v>
       </c>
       <c r="C43">
-        <v>162</v>
+        <v>339</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C44">
-        <v>162</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C45">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C46">
-        <v>153</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="C47">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C48">
-        <v>147</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>109</v>
       </c>
       <c r="C49">
-        <v>147</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C50">
-        <v>147</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>145</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{10F88A25-3109-4560-BC52-6B05C997EE06}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14552,8 +14582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C9A92E-4F85-41BB-8EBB-810FED829DA1}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14562,8 +14592,8 @@
     <col min="2" max="2" width="13.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="32" customWidth="1"/>
-    <col min="6" max="8" width="6.77734375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="31" customWidth="1"/>
+    <col min="6" max="8" width="6.77734375" style="26" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
@@ -14580,7 +14610,7 @@
       <c r="D1" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="28"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="21" t="s">
         <v>160</v>
       </c>
@@ -14592,7 +14622,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="18">
@@ -14604,7 +14634,7 @@
       <c r="D2" s="18">
         <v>89</v>
       </c>
-      <c r="E2" s="29"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="22">
         <v>381</v>
       </c>
@@ -14616,2139 +14646,2139 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="16">
-        <v>238</v>
+      <c r="A3" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="18">
+        <v>460</v>
       </c>
       <c r="C3" s="18">
-        <v>497</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="22">
-        <v>207</v>
-      </c>
-      <c r="G3" s="23">
-        <v>164</v>
-      </c>
-      <c r="H3" s="22">
-        <v>598</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="D3" s="18">
+        <v>72</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="23">
+        <v>111</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
-        <v>13</v>
+      <c r="A4" s="34" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="16">
-        <v>176</v>
-      </c>
-      <c r="C4" s="18">
-        <v>445</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="29"/>
+        <v>173</v>
+      </c>
+      <c r="C4" s="16">
+        <v>220</v>
+      </c>
+      <c r="D4" s="18">
+        <v>59</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="22">
-        <v>222</v>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23">
-        <v>278</v>
+        <v>192</v>
+      </c>
+      <c r="G4" s="22">
+        <v>250</v>
+      </c>
+      <c r="H4" s="22">
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="16">
+        <v>203</v>
+      </c>
       <c r="C5" s="18">
-        <v>420</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="29"/>
+        <v>367</v>
+      </c>
+      <c r="D5" s="18">
+        <v>58</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="16">
-        <v>203</v>
-      </c>
-      <c r="C6" s="18">
-        <v>367</v>
-      </c>
+      <c r="A6" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="18">
-        <v>58</v>
-      </c>
-      <c r="E6" s="29"/>
+        <v>54</v>
+      </c>
+      <c r="E6" s="28"/>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="16">
-        <v>212</v>
-      </c>
-      <c r="C7" s="18">
-        <v>362</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="22">
-        <v>183</v>
-      </c>
-      <c r="G7" s="23">
-        <v>196</v>
+      <c r="A7" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="18">
+        <v>330</v>
+      </c>
+      <c r="C7" s="16">
+        <v>222</v>
+      </c>
+      <c r="D7" s="18">
+        <v>51</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="23">
+        <v>129</v>
+      </c>
+      <c r="G7" s="22">
+        <v>206</v>
       </c>
       <c r="H7" s="22">
-        <v>628</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="18">
-        <v>460</v>
-      </c>
-      <c r="C8" s="18">
-        <v>361</v>
+      <c r="A8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16">
+        <v>168</v>
+      </c>
+      <c r="C8" s="16">
+        <v>213</v>
       </c>
       <c r="D8" s="18">
-        <v>72</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="23">
-        <v>111</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="16">
+        <v>218</v>
+      </c>
+      <c r="C9" s="16">
+        <v>225</v>
+      </c>
+      <c r="D9" s="18">
         <v>48</v>
       </c>
-      <c r="B9" s="18">
-        <v>474</v>
-      </c>
-      <c r="C9" s="18">
-        <v>346</v>
-      </c>
-      <c r="D9" s="18">
-        <v>40</v>
-      </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="22">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="G9" s="22">
-        <v>288</v>
+        <v>218</v>
       </c>
       <c r="H9" s="22">
-        <v>549</v>
+        <v>680</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="18">
+        <v>295</v>
+      </c>
+      <c r="C10" s="18">
+        <v>236</v>
+      </c>
+      <c r="D10" s="18">
         <v>46</v>
       </c>
-      <c r="B10" s="18">
-        <v>435</v>
-      </c>
-      <c r="C10" s="18">
-        <v>320</v>
-      </c>
-      <c r="D10" s="16">
-        <v>24</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="22">
-        <v>178</v>
-      </c>
-      <c r="G10" s="23">
-        <v>168</v>
-      </c>
-      <c r="H10" s="23">
-        <v>190</v>
+      <c r="E10" s="28"/>
+      <c r="F10" s="23">
+        <v>135</v>
+      </c>
+      <c r="G10" s="22">
+        <v>212</v>
+      </c>
+      <c r="H10" s="22">
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>180</v>
+      <c r="A11" s="32" t="s">
+        <v>121</v>
       </c>
       <c r="B11" s="16"/>
-      <c r="C11" s="18">
-        <v>306</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="18">
+        <v>45</v>
+      </c>
+      <c r="E11" s="28"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="18">
+        <v>369</v>
+      </c>
+      <c r="C12" s="16">
+        <v>167</v>
+      </c>
+      <c r="D12" s="18">
         <v>44</v>
       </c>
-      <c r="B12" s="18">
-        <v>365</v>
-      </c>
-      <c r="C12" s="18">
-        <v>299</v>
-      </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="29"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="22">
+        <v>149</v>
+      </c>
+      <c r="G12" s="22">
+        <v>276</v>
+      </c>
+      <c r="H12" s="23">
         <v>213</v>
       </c>
-      <c r="G12" s="22">
-        <v>338</v>
-      </c>
-      <c r="H12" s="23">
-        <v>204</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="18">
-        <v>293</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="22">
+      <c r="A13" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="16">
+        <v>213</v>
+      </c>
+      <c r="C13" s="16">
+        <v>177</v>
+      </c>
+      <c r="D13" s="18">
+        <v>44</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16">
+        <v>208</v>
+      </c>
+      <c r="D14" s="18">
+        <v>44</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="23">
+        <v>102</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="37">
+        <v>281</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="37">
+        <v>41</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24">
+        <v>152</v>
+      </c>
+      <c r="H15" s="24">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="16">
         <v>189</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="C16" s="16">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18">
+        <v>41</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="18">
+        <v>474</v>
+      </c>
+      <c r="C17" s="18">
+        <v>346</v>
+      </c>
+      <c r="D17" s="18">
         <v>40</v>
       </c>
-      <c r="B14" s="18">
-        <v>301</v>
-      </c>
-      <c r="C14" s="18">
-        <v>274</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="22">
-        <v>185</v>
-      </c>
-      <c r="G14" s="23">
-        <v>178</v>
-      </c>
-      <c r="H14" s="23">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18">
-        <v>254</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="18">
-        <v>295</v>
-      </c>
-      <c r="C16" s="18">
-        <v>236</v>
-      </c>
-      <c r="D16" s="18">
-        <v>46</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="23">
-        <v>135</v>
-      </c>
-      <c r="G16" s="22">
+      <c r="E17" s="28"/>
+      <c r="F17" s="22">
+        <v>195</v>
+      </c>
+      <c r="G17" s="22">
+        <v>288</v>
+      </c>
+      <c r="H17" s="22">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16">
+        <v>38</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="16">
         <v>212</v>
       </c>
-      <c r="H16" s="22">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" s="16">
-        <v>218</v>
-      </c>
-      <c r="C17" s="16">
-        <v>225</v>
-      </c>
-      <c r="D17" s="18">
-        <v>48</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="22">
-        <v>200</v>
-      </c>
-      <c r="G17" s="22">
-        <v>218</v>
-      </c>
-      <c r="H17" s="22">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="18">
-        <v>330</v>
-      </c>
-      <c r="C18" s="16">
-        <v>222</v>
-      </c>
-      <c r="D18" s="18">
-        <v>51</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="23">
-        <v>129</v>
-      </c>
-      <c r="G18" s="22">
-        <v>206</v>
-      </c>
-      <c r="H18" s="22">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="16">
-        <v>173</v>
-      </c>
       <c r="C19" s="16">
-        <v>220</v>
-      </c>
-      <c r="D19" s="18">
-        <v>59</v>
-      </c>
-      <c r="E19" s="29"/>
+        <v>201</v>
+      </c>
+      <c r="D19" s="16">
+        <v>37</v>
+      </c>
+      <c r="E19" s="28"/>
       <c r="F19" s="22">
-        <v>192</v>
-      </c>
-      <c r="G19" s="22">
-        <v>250</v>
+        <v>167</v>
+      </c>
+      <c r="G19" s="23">
+        <v>202</v>
       </c>
       <c r="H19" s="22">
-        <v>626</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16">
-        <v>217</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="29"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="16">
+        <v>174</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <v>37</v>
+      </c>
+      <c r="E20" s="28"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="23">
-        <v>168</v>
-      </c>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="B21" s="16">
+        <v>162</v>
+      </c>
       <c r="C21" s="16">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="D21" s="16">
-        <v>24</v>
-      </c>
-      <c r="E21" s="29"/>
+        <v>37</v>
+      </c>
+      <c r="E21" s="28"/>
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="16">
-        <v>168</v>
-      </c>
-      <c r="C22" s="16">
-        <v>213</v>
-      </c>
-      <c r="D22" s="18">
-        <v>49</v>
-      </c>
-      <c r="E22" s="29"/>
+      <c r="A22" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
+        <v>37</v>
+      </c>
+      <c r="E22" s="28"/>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>81</v>
+      <c r="A23" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="B23" s="16"/>
-      <c r="C23" s="16">
-        <v>208</v>
-      </c>
-      <c r="D23" s="18">
-        <v>44</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="23">
-        <v>102</v>
-      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16">
+        <v>36</v>
+      </c>
+      <c r="E23" s="28"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="22">
-        <v>377</v>
-      </c>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="B24" s="16"/>
-      <c r="C24" s="16">
-        <v>202</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="29"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16">
+        <v>36</v>
+      </c>
+      <c r="E24" s="28"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="16">
-        <v>212</v>
-      </c>
-      <c r="C25" s="16">
-        <v>201</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="16">
-        <v>37</v>
-      </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="22">
-        <v>167</v>
-      </c>
-      <c r="G25" s="23">
-        <v>202</v>
-      </c>
-      <c r="H25" s="22">
-        <v>378</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B26" s="16"/>
+      <c r="A26" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="18">
+        <v>293</v>
+      </c>
       <c r="C26" s="16">
-        <v>198</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="D26" s="16">
+        <v>33</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="23">
+        <v>127</v>
+      </c>
+      <c r="G26" s="22">
+        <v>272</v>
+      </c>
+      <c r="H26" s="23">
+        <v>217</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16">
-        <v>194</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="22">
-        <v>168</v>
+        <v>147</v>
+      </c>
+      <c r="D27" s="16">
+        <v>31</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="23">
+        <v>144</v>
       </c>
       <c r="G27" s="23">
-        <v>140</v>
-      </c>
-      <c r="H27" s="23">
-        <v>256</v>
+        <v>174</v>
+      </c>
+      <c r="H27" s="22">
+        <v>796</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="16">
-        <v>195</v>
-      </c>
-      <c r="C28" s="16">
-        <v>189</v>
-      </c>
-      <c r="D28" s="16"/>
+      <c r="A28" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20">
+        <v>31</v>
+      </c>
       <c r="E28" s="29"/>
-      <c r="F28" s="23">
-        <v>102</v>
-      </c>
-      <c r="G28" s="23">
-        <v>128</v>
-      </c>
-      <c r="H28" s="23">
-        <v>180</v>
-      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="16">
-        <v>180</v>
-      </c>
-      <c r="C29" s="16">
-        <v>185</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="16">
-        <v>24</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="23">
-        <v>103</v>
-      </c>
-      <c r="G29" s="23">
-        <v>140</v>
-      </c>
-      <c r="H29" s="23">
-        <v>297</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16">
-        <v>177</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="29"/>
+      <c r="A30" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="18">
+        <v>283</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16">
+        <v>28</v>
+      </c>
+      <c r="E30" s="28"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23"/>
       <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="16">
-        <v>213</v>
-      </c>
-      <c r="C31" s="16">
-        <v>177</v>
-      </c>
-      <c r="D31" s="18">
-        <v>44</v>
-      </c>
-      <c r="E31" s="29"/>
+      <c r="A31" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
+        <v>28</v>
+      </c>
+      <c r="E31" s="28"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="18">
-        <v>304</v>
+        <v>19</v>
+      </c>
+      <c r="B32" s="16">
+        <v>192</v>
       </c>
       <c r="C32" s="16">
         <v>170</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="23"/>
+      <c r="D32" s="16">
+        <v>27</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="23">
+        <v>100</v>
+      </c>
       <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="H32" s="23">
+        <v>216</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" s="16">
-        <v>192</v>
-      </c>
-      <c r="C33" s="16">
-        <v>170</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C33" s="16"/>
       <c r="D33" s="16">
         <v>27</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="23">
-        <v>100</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23">
-        <v>216</v>
-      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23">
+        <v>142</v>
+      </c>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B34" s="16"/>
-      <c r="C34" s="16">
-        <v>168</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="29"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16">
+        <v>27</v>
+      </c>
+      <c r="E34" s="28"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="H34" s="23">
-        <v>241</v>
-      </c>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="16">
-        <v>189</v>
-      </c>
-      <c r="C35" s="16">
-        <v>167</v>
-      </c>
-      <c r="D35" s="18">
-        <v>41</v>
-      </c>
-      <c r="E35" s="29"/>
+        <v>111</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16">
+        <v>26</v>
+      </c>
+      <c r="E35" s="28"/>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
-      <c r="H35" s="23">
-        <v>207</v>
-      </c>
+      <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="18">
-        <v>369</v>
-      </c>
-      <c r="C36" s="16">
-        <v>167</v>
-      </c>
-      <c r="D36" s="18">
-        <v>44</v>
-      </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="22">
-        <v>149</v>
-      </c>
-      <c r="G36" s="22">
-        <v>276</v>
-      </c>
-      <c r="H36" s="23">
-        <v>213</v>
-      </c>
+      <c r="A36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16">
+        <v>26</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="16">
-        <v>162</v>
-      </c>
-      <c r="C37" s="16">
-        <v>165</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="16">
-        <v>37</v>
-      </c>
-      <c r="E37" s="29"/>
+        <v>26</v>
+      </c>
+      <c r="E37" s="28"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="18">
-        <v>331</v>
-      </c>
-      <c r="C38" s="16">
-        <v>162</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="23">
-        <v>136</v>
-      </c>
-      <c r="G38" s="22">
-        <v>220</v>
-      </c>
-      <c r="H38" s="22">
-        <v>371</v>
-      </c>
+      <c r="A38" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16">
+        <v>26</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16">
-        <v>162</v>
-      </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="B39" s="16">
+        <v>160</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16">
+        <v>25</v>
+      </c>
+      <c r="E39" s="28"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B40" s="16"/>
-      <c r="C40" s="16">
-        <v>159</v>
-      </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="23">
-        <v>133</v>
-      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16">
+        <v>25</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="23"/>
-      <c r="H40" s="23">
-        <v>205</v>
-      </c>
+      <c r="H40" s="23"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="B41" s="16"/>
-      <c r="C41" s="16">
-        <v>153</v>
-      </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="29"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16">
+        <v>25</v>
+      </c>
+      <c r="E41" s="28"/>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="16">
-        <v>160</v>
-      </c>
-      <c r="C42" s="16">
-        <v>153</v>
-      </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="29"/>
+        <v>106</v>
+      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16">
+        <v>25</v>
+      </c>
+      <c r="E42" s="28"/>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
       <c r="H42" s="23"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16">
-        <v>147</v>
-      </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="23">
-        <v>100</v>
-      </c>
-      <c r="G43" s="23"/>
+      <c r="A43" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="18">
+        <v>435</v>
+      </c>
+      <c r="C43" s="18">
+        <v>320</v>
+      </c>
+      <c r="D43" s="16">
+        <v>24</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="22">
+        <v>178</v>
+      </c>
+      <c r="G43" s="23">
+        <v>168</v>
+      </c>
       <c r="H43" s="23">
-        <v>225</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B44" s="16"/>
+        <v>14</v>
+      </c>
+      <c r="B44" s="16">
+        <v>180</v>
+      </c>
       <c r="C44" s="16">
-        <v>147</v>
-      </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
+        <v>185</v>
+      </c>
+      <c r="D44" s="16">
+        <v>24</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="23">
+        <v>103</v>
+      </c>
+      <c r="G44" s="23">
+        <v>140</v>
+      </c>
+      <c r="H44" s="23">
+        <v>297</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="16">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="D45" s="16">
-        <v>31</v>
-      </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="23">
-        <v>144</v>
-      </c>
-      <c r="G45" s="23">
-        <v>174</v>
-      </c>
-      <c r="H45" s="22">
-        <v>796</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="18">
-        <v>293</v>
-      </c>
-      <c r="C46" s="16">
-        <v>145</v>
-      </c>
+      <c r="A46" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="16">
-        <v>33</v>
-      </c>
-      <c r="E46" s="29"/>
-      <c r="F46" s="23">
-        <v>127</v>
-      </c>
-      <c r="G46" s="22">
-        <v>272</v>
-      </c>
-      <c r="H46" s="23">
-        <v>217</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16">
-        <v>26</v>
-      </c>
-      <c r="E47" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="E47" s="28"/>
       <c r="F47" s="23"/>
       <c r="G47" s="23"/>
       <c r="H47" s="23"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="A48" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20">
+        <v>24</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="22">
-        <v>218</v>
-      </c>
-      <c r="H48" s="23"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
+      <c r="A49" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="18">
+        <v>365</v>
+      </c>
+      <c r="C49" s="18">
+        <v>299</v>
+      </c>
       <c r="D49" s="16"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="22">
+        <v>213</v>
+      </c>
+      <c r="G49" s="22">
+        <v>338</v>
+      </c>
       <c r="H49" s="23">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="18">
+        <v>331</v>
+      </c>
+      <c r="C50" s="16">
+        <v>162</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="23">
+        <v>136</v>
+      </c>
+      <c r="G50" s="22">
         <v>220</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16">
-        <v>36</v>
-      </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
+      <c r="H50" s="22">
+        <v>371</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="16">
-        <v>225</v>
-      </c>
-      <c r="C51" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="B51" s="18">
+        <v>304</v>
+      </c>
+      <c r="C51" s="16">
+        <v>170</v>
+      </c>
       <c r="D51" s="16"/>
-      <c r="E51" s="29"/>
+      <c r="E51" s="28"/>
       <c r="F51" s="23"/>
       <c r="G51" s="23"/>
       <c r="H51" s="23"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
+      <c r="A52" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="18">
+        <v>301</v>
+      </c>
+      <c r="C52" s="18">
+        <v>274</v>
+      </c>
       <c r="D52" s="16"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="23"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="22">
+        <v>185</v>
+      </c>
       <c r="G52" s="23">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="H52" s="23">
-        <v>205</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="16"/>
+      <c r="A53" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="18">
+        <v>280</v>
+      </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="29"/>
+      <c r="E53" s="28"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="23">
-        <v>126</v>
-      </c>
-      <c r="H53" s="22">
-        <v>334</v>
-      </c>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="16"/>
+      <c r="A54" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="16">
+        <v>278</v>
+      </c>
       <c r="C54" s="16"/>
-      <c r="D54" s="16">
-        <v>24</v>
-      </c>
-      <c r="E54" s="29"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="28"/>
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="23"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="16"/>
+      <c r="A55" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="18">
+        <v>260</v>
+      </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="23">
-        <v>110</v>
-      </c>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23">
-        <v>176</v>
-      </c>
+      <c r="E55" s="28"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23">
+        <v>158</v>
+      </c>
+      <c r="H55" s="23"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="B56" s="16">
+        <v>249</v>
+      </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23">
-        <v>144</v>
-      </c>
-      <c r="H56" s="23"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="22">
+        <v>187</v>
+      </c>
+      <c r="G56" s="22">
+        <v>292</v>
+      </c>
+      <c r="H56" s="22">
+        <v>468</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
+      <c r="A57" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="16">
+        <v>238</v>
+      </c>
+      <c r="C57" s="18">
+        <v>497</v>
+      </c>
       <c r="D57" s="16"/>
-      <c r="E57" s="29"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="22">
-        <v>146</v>
-      </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23"/>
+        <v>207</v>
+      </c>
+      <c r="G57" s="23">
+        <v>164</v>
+      </c>
+      <c r="H57" s="22">
+        <v>598</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="16"/>
+        <v>28</v>
+      </c>
+      <c r="B58" s="16">
+        <v>225</v>
+      </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
-      <c r="E58" s="29"/>
+      <c r="E58" s="28"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="23">
-        <v>168</v>
-      </c>
+      <c r="G58" s="23"/>
       <c r="H58" s="23"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
+      <c r="A59" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="16">
+        <v>212</v>
+      </c>
+      <c r="C59" s="18">
+        <v>362</v>
+      </c>
       <c r="D59" s="16"/>
-      <c r="E59" s="29"/>
+      <c r="E59" s="28"/>
       <c r="F59" s="22">
-        <v>150</v>
-      </c>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
+        <v>183</v>
+      </c>
+      <c r="G59" s="23">
+        <v>196</v>
+      </c>
+      <c r="H59" s="22">
+        <v>628</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="16"/>
+        <v>23</v>
+      </c>
+      <c r="B60" s="16">
+        <v>207</v>
+      </c>
       <c r="C60" s="16"/>
-      <c r="D60" s="16">
-        <v>28</v>
-      </c>
-      <c r="E60" s="29"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="28"/>
       <c r="F60" s="23"/>
       <c r="G60" s="23"/>
       <c r="H60" s="23"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" s="16"/>
+        <v>22</v>
+      </c>
+      <c r="B61" s="16">
+        <v>206</v>
+      </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="23">
-        <v>123</v>
-      </c>
+      <c r="E61" s="28"/>
+      <c r="F61" s="23"/>
       <c r="G61" s="23"/>
-      <c r="H61" s="23">
-        <v>170</v>
-      </c>
+      <c r="H61" s="23"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16">
-        <v>38</v>
-      </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="B62" s="16">
+        <v>195</v>
+      </c>
+      <c r="C62" s="16">
+        <v>189</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="23">
+        <v>102</v>
+      </c>
+      <c r="G62" s="23">
+        <v>128</v>
+      </c>
+      <c r="H62" s="23">
+        <v>180</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="B63" s="16">
+        <v>184</v>
+      </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16"/>
-      <c r="E63" s="29"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="23">
-        <v>140</v>
-      </c>
-      <c r="G63" s="23"/>
+        <v>101</v>
+      </c>
+      <c r="G63" s="23">
+        <v>148</v>
+      </c>
       <c r="H63" s="23"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
+      <c r="A64" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="16">
+        <v>176</v>
+      </c>
+      <c r="C64" s="18">
+        <v>445</v>
+      </c>
       <c r="D64" s="16"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="23"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="22">
+        <v>222</v>
+      </c>
       <c r="G64" s="23"/>
-      <c r="H64" s="22">
-        <v>420</v>
+      <c r="H64" s="23">
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B65" s="16">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="C65" s="16"/>
-      <c r="D65" s="16">
-        <v>25</v>
-      </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="23"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="23">
+        <v>98</v>
+      </c>
+      <c r="G65" s="22">
+        <v>312</v>
+      </c>
+      <c r="H65" s="23">
+        <v>192</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16">
-        <v>25</v>
-      </c>
+      <c r="A66" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="20">
+        <v>172</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
       <c r="E66" s="29"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B67" s="16">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C67" s="16"/>
       <c r="D67" s="16"/>
-      <c r="E67" s="29"/>
+      <c r="E67" s="28"/>
       <c r="F67" s="23">
-        <v>105</v>
-      </c>
-      <c r="G67" s="22">
-        <v>484</v>
+        <v>95</v>
+      </c>
+      <c r="G67" s="23">
+        <v>192</v>
       </c>
       <c r="H67" s="23"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="B68" s="16">
+        <v>170</v>
+      </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="23">
-        <v>111</v>
-      </c>
-      <c r="G68" s="22">
-        <v>300</v>
+      <c r="E68" s="28"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23">
+        <v>134</v>
       </c>
       <c r="H68" s="23"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B69" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="B69" s="16">
+        <v>162</v>
+      </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
-      <c r="E69" s="29"/>
+      <c r="E69" s="28"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="23">
-        <v>128</v>
-      </c>
+      <c r="G69" s="23"/>
       <c r="H69" s="23"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="B70" s="16">
+        <v>160</v>
+      </c>
+      <c r="C70" s="16">
+        <v>153</v>
+      </c>
       <c r="D70" s="16"/>
-      <c r="E70" s="29"/>
+      <c r="E70" s="28"/>
       <c r="F70" s="23"/>
       <c r="G70" s="23"/>
-      <c r="H70" s="23">
-        <v>236</v>
-      </c>
+      <c r="H70" s="23"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B71" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="B71" s="20">
+        <v>158</v>
+      </c>
       <c r="C71" s="20"/>
       <c r="D71" s="20"/>
-      <c r="E71" s="30"/>
+      <c r="E71" s="29"/>
       <c r="F71" s="24"/>
-      <c r="G71" s="24">
-        <v>124</v>
-      </c>
+      <c r="G71" s="24"/>
       <c r="H71" s="24"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B72" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="B72" s="16">
+        <v>157</v>
+      </c>
       <c r="C72" s="16"/>
       <c r="D72" s="16"/>
-      <c r="E72" s="29"/>
+      <c r="E72" s="28"/>
       <c r="F72" s="23">
-        <v>143</v>
-      </c>
-      <c r="G72" s="23"/>
+        <v>105</v>
+      </c>
+      <c r="G72" s="22">
+        <v>484</v>
+      </c>
       <c r="H72" s="23"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B73" s="18">
-        <v>280</v>
-      </c>
-      <c r="C73" s="16"/>
+      <c r="A73" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="16"/>
+      <c r="C73" s="18">
+        <v>420</v>
+      </c>
       <c r="D73" s="16"/>
-      <c r="E73" s="29"/>
+      <c r="E73" s="28"/>
       <c r="F73" s="23"/>
       <c r="G73" s="23"/>
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="15" t="s">
-        <v>85</v>
+      <c r="A74" s="32" t="s">
+        <v>180</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
+      <c r="C74" s="18">
+        <v>306</v>
+      </c>
       <c r="D74" s="16"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="23">
-        <v>126</v>
-      </c>
+      <c r="E74" s="28"/>
+      <c r="F74" s="23"/>
       <c r="G74" s="23"/>
       <c r="H74" s="23"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="16">
-        <v>207</v>
-      </c>
-      <c r="C75" s="16"/>
+      <c r="A75" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="16"/>
+      <c r="C75" s="18">
+        <v>293</v>
+      </c>
       <c r="D75" s="16"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="23"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="22">
+        <v>189</v>
+      </c>
       <c r="G75" s="23"/>
-      <c r="H75" s="23"/>
+      <c r="H75" s="22">
+        <v>499</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="15" t="s">
-        <v>57</v>
+      <c r="A76" s="32" t="s">
+        <v>169</v>
       </c>
       <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
+      <c r="C76" s="18">
+        <v>254</v>
+      </c>
       <c r="D76" s="16"/>
-      <c r="E76" s="29"/>
-      <c r="F76" s="23">
-        <v>95</v>
-      </c>
-      <c r="G76" s="23">
-        <v>140</v>
-      </c>
+      <c r="E76" s="28"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="23"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="18">
-        <v>260</v>
-      </c>
-      <c r="C77" s="16"/>
+      <c r="A77" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16">
+        <v>217</v>
+      </c>
       <c r="D77" s="16"/>
-      <c r="E77" s="29"/>
+      <c r="E77" s="28"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="23">
-        <v>158</v>
-      </c>
-      <c r="H77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23">
+        <v>168</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="24">
-        <v>94</v>
-      </c>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
+      <c r="A78" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16">
+        <v>202</v>
+      </c>
+      <c r="D78" s="16"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
+      <c r="C79" s="16">
+        <v>198</v>
+      </c>
       <c r="D79" s="16"/>
-      <c r="E79" s="29"/>
+      <c r="E79" s="28"/>
       <c r="F79" s="23"/>
       <c r="G79" s="23"/>
-      <c r="H79" s="23">
-        <v>174</v>
-      </c>
+      <c r="H79" s="23"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80" s="16">
-        <v>162</v>
-      </c>
-      <c r="C80" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16">
+        <v>194</v>
+      </c>
       <c r="D80" s="16"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="23"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="22">
+        <v>168</v>
+      </c>
+      <c r="G80" s="23">
+        <v>140</v>
+      </c>
+      <c r="H80" s="23">
+        <v>256</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
+      <c r="C81" s="16">
+        <v>177</v>
+      </c>
       <c r="D81" s="16"/>
-      <c r="E81" s="29"/>
+      <c r="E81" s="28"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="23">
-        <v>180</v>
-      </c>
+      <c r="G81" s="23"/>
       <c r="H81" s="23"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
+      <c r="C82" s="16">
+        <v>168</v>
+      </c>
       <c r="D82" s="16"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="23">
-        <v>132</v>
-      </c>
+      <c r="E82" s="28"/>
+      <c r="F82" s="23"/>
       <c r="G82" s="23"/>
-      <c r="H82" s="22">
-        <v>384</v>
+      <c r="H82" s="23">
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
+      <c r="C83" s="16">
+        <v>162</v>
+      </c>
       <c r="D83" s="16"/>
-      <c r="E83" s="29"/>
+      <c r="E83" s="28"/>
       <c r="F83" s="23"/>
       <c r="G83" s="23"/>
-      <c r="H83" s="23">
-        <v>251</v>
-      </c>
+      <c r="H83" s="23"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16">
-        <v>27</v>
-      </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="23"/>
+      <c r="C84" s="16">
+        <v>159</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="23">
+        <v>133</v>
+      </c>
       <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
+      <c r="H84" s="23">
+        <v>205</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" s="16">
-        <v>171</v>
-      </c>
-      <c r="C85" s="16"/>
+        <v>175</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16">
+        <v>153</v>
+      </c>
       <c r="D85" s="16"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="23">
-        <v>95</v>
-      </c>
-      <c r="G85" s="23">
-        <v>192</v>
-      </c>
+      <c r="E85" s="28"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
       <c r="H85" s="23"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B86" s="16"/>
-      <c r="C86" s="16"/>
+      <c r="C86" s="16">
+        <v>147</v>
+      </c>
       <c r="D86" s="16"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23">
-        <v>156</v>
-      </c>
-      <c r="H86" s="23"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="23">
+        <v>100</v>
+      </c>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23">
+        <v>225</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
+      <c r="C87" s="16">
+        <v>147</v>
+      </c>
       <c r="D87" s="16"/>
-      <c r="E87" s="29"/>
+      <c r="E87" s="28"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="23">
-        <v>140</v>
-      </c>
+      <c r="G87" s="23"/>
       <c r="H87" s="23"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
-      <c r="D88" s="16">
-        <v>24</v>
-      </c>
-      <c r="E88" s="29"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="28"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="23"/>
+      <c r="G88" s="22">
+        <v>218</v>
+      </c>
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="33" t="s">
-        <v>122</v>
+      <c r="A89" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="B89" s="16"/>
       <c r="C89" s="16"/>
-      <c r="D89" s="18">
-        <v>54</v>
-      </c>
-      <c r="E89" s="29"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="28"/>
       <c r="F89" s="23"/>
       <c r="G89" s="23"/>
-      <c r="H89" s="23"/>
+      <c r="H89" s="23">
+        <v>220</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B90" s="16"/>
       <c r="C90" s="16"/>
       <c r="D90" s="16"/>
-      <c r="E90" s="29"/>
+      <c r="E90" s="28"/>
       <c r="F90" s="23"/>
       <c r="G90" s="23">
-        <v>166</v>
-      </c>
-      <c r="H90" s="23"/>
+        <v>164</v>
+      </c>
+      <c r="H90" s="23">
+        <v>205</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
-      <c r="D91" s="16">
-        <v>25</v>
-      </c>
-      <c r="E91" s="29"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="28"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="23"/>
-      <c r="H91" s="23"/>
+      <c r="G91" s="23">
+        <v>126</v>
+      </c>
+      <c r="H91" s="22">
+        <v>334</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B92" s="16">
-        <v>189</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B92" s="16"/>
       <c r="C92" s="16"/>
-      <c r="D92" s="16">
-        <v>27</v>
-      </c>
-      <c r="E92" s="29"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="23">
-        <v>142</v>
-      </c>
-      <c r="H92" s="23"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="23">
+        <v>110</v>
+      </c>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23">
+        <v>176</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B93" s="16">
-        <v>170</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B93" s="16"/>
       <c r="C93" s="16"/>
       <c r="D93" s="16"/>
-      <c r="E93" s="29"/>
+      <c r="E93" s="28"/>
       <c r="F93" s="23"/>
       <c r="G93" s="23">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="H93" s="23"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="24"/>
-      <c r="H94" s="24">
-        <v>171</v>
-      </c>
+      <c r="A94" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="22">
+        <v>146</v>
+      </c>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B95" s="16"/>
       <c r="C95" s="16"/>
       <c r="D95" s="16"/>
-      <c r="E95" s="29"/>
+      <c r="E95" s="28"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="22">
-        <v>210</v>
+      <c r="G95" s="23">
+        <v>168</v>
       </c>
       <c r="H95" s="23"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="D96" s="16"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="23">
-        <v>132</v>
-      </c>
+      <c r="E96" s="28"/>
+      <c r="F96" s="22">
+        <v>150</v>
+      </c>
+      <c r="G96" s="23"/>
       <c r="H96" s="23"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B97" s="16">
-        <v>174</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B97" s="16"/>
       <c r="C97" s="16"/>
       <c r="D97" s="16"/>
-      <c r="E97" s="29"/>
+      <c r="E97" s="28"/>
       <c r="F97" s="23">
-        <v>98</v>
-      </c>
-      <c r="G97" s="22">
-        <v>312</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="G97" s="23"/>
       <c r="H97" s="23">
-        <v>192</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B98" s="16"/>
       <c r="C98" s="16"/>
-      <c r="D98" s="16">
-        <v>37</v>
-      </c>
-      <c r="E98" s="29"/>
-      <c r="F98" s="23"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="23">
+        <v>140</v>
+      </c>
       <c r="G98" s="23"/>
       <c r="H98" s="23"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="B99" s="16"/>
       <c r="C99" s="16"/>
       <c r="D99" s="16"/>
-      <c r="E99" s="29"/>
-      <c r="F99" s="22">
-        <v>154</v>
-      </c>
+      <c r="E99" s="28"/>
+      <c r="F99" s="23"/>
       <c r="G99" s="23"/>
-      <c r="H99" s="23"/>
+      <c r="H99" s="22">
+        <v>420</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B100" s="16"/>
       <c r="C100" s="16"/>
-      <c r="D100" s="16">
-        <v>26</v>
-      </c>
-      <c r="E100" s="29"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="23">
+        <v>111</v>
+      </c>
+      <c r="G100" s="22">
+        <v>300</v>
+      </c>
       <c r="H100" s="23"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
-        <v>128</v>
+        <v>54</v>
       </c>
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
-      <c r="E101" s="29"/>
+      <c r="E101" s="28"/>
       <c r="F101" s="23"/>
-      <c r="G101" s="23"/>
-      <c r="H101" s="23">
-        <v>179</v>
-      </c>
+      <c r="G101" s="23">
+        <v>128</v>
+      </c>
+      <c r="H101" s="23"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="23">
-        <v>97</v>
-      </c>
+      <c r="E102" s="28"/>
+      <c r="F102" s="23"/>
       <c r="G102" s="23"/>
       <c r="H102" s="23">
-        <v>192</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B103" s="16"/>
-      <c r="C103" s="16"/>
-      <c r="D103" s="16"/>
+      <c r="A103" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="20"/>
       <c r="E103" s="29"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="22">
-        <v>204</v>
-      </c>
-      <c r="H103" s="23"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24">
+        <v>124</v>
+      </c>
+      <c r="H103" s="24"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" s="20">
-        <v>158</v>
-      </c>
-      <c r="C104" s="20"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="30"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
+      <c r="A104" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="16"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="23">
+        <v>143</v>
+      </c>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B105" s="16">
-        <v>184</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B105" s="16"/>
       <c r="C105" s="16"/>
       <c r="D105" s="16"/>
-      <c r="E105" s="29"/>
+      <c r="E105" s="28"/>
       <c r="F105" s="23">
-        <v>101</v>
-      </c>
-      <c r="G105" s="23">
-        <v>148</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G105" s="23"/>
       <c r="H105" s="23"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="B106" s="16"/>
       <c r="C106" s="16"/>
       <c r="D106" s="16"/>
-      <c r="E106" s="29"/>
+      <c r="E106" s="28"/>
       <c r="F106" s="23">
-        <v>116</v>
-      </c>
-      <c r="G106" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G106" s="23">
+        <v>140</v>
+      </c>
       <c r="H106" s="23"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B107" s="16"/>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
+      <c r="A107" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B107" s="20"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
       <c r="E107" s="29"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="23">
-        <v>148</v>
-      </c>
-      <c r="H107" s="23"/>
+      <c r="F107" s="24">
+        <v>94</v>
+      </c>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="15" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B108" s="16"/>
       <c r="C108" s="16"/>
-      <c r="D108" s="16">
-        <v>26</v>
-      </c>
-      <c r="E108" s="29"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="28"/>
       <c r="F108" s="23"/>
       <c r="G108" s="23"/>
-      <c r="H108" s="23"/>
+      <c r="H108" s="23">
+        <v>174</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B109" s="20"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="20">
-        <v>24</v>
-      </c>
-      <c r="E109" s="30"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
-      <c r="H109" s="24"/>
+      <c r="A109" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23">
+        <v>180</v>
+      </c>
+      <c r="H109" s="23"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B110" s="16">
-        <v>174</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B110" s="16"/>
       <c r="C110" s="16"/>
-      <c r="D110" s="16">
-        <v>37</v>
-      </c>
-      <c r="E110" s="29"/>
-      <c r="F110" s="23"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="23">
+        <v>132</v>
+      </c>
       <c r="G110" s="23"/>
-      <c r="H110" s="23"/>
+      <c r="H110" s="22">
+        <v>384</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B111" s="16"/>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
-      <c r="E111" s="29"/>
+      <c r="E111" s="28"/>
       <c r="F111" s="23"/>
-      <c r="G111" s="23">
-        <v>200</v>
-      </c>
-      <c r="H111" s="23"/>
+      <c r="G111" s="23"/>
+      <c r="H111" s="23">
+        <v>251</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B112" s="16"/>
       <c r="C112" s="16"/>
-      <c r="D112" s="16">
-        <v>25</v>
-      </c>
-      <c r="E112" s="29"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="28"/>
       <c r="F112" s="23"/>
-      <c r="G112" s="23"/>
+      <c r="G112" s="23">
+        <v>156</v>
+      </c>
       <c r="H112" s="23"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="B113" s="16"/>
       <c r="C113" s="16"/>
-      <c r="D113" s="16">
-        <v>36</v>
-      </c>
-      <c r="E113" s="29"/>
+      <c r="D113" s="16"/>
+      <c r="E113" s="28"/>
       <c r="F113" s="23"/>
-      <c r="G113" s="23"/>
+      <c r="G113" s="23">
+        <v>140</v>
+      </c>
       <c r="H113" s="23"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B114" s="16">
-        <v>278</v>
-      </c>
+      <c r="A114" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B114" s="16"/>
       <c r="C114" s="16"/>
       <c r="D114" s="16"/>
-      <c r="E114" s="29"/>
+      <c r="E114" s="28"/>
       <c r="F114" s="23"/>
-      <c r="G114" s="23"/>
+      <c r="G114" s="23">
+        <v>166</v>
+      </c>
       <c r="H114" s="23"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B115" s="18">
-        <v>283</v>
-      </c>
-      <c r="C115" s="16"/>
-      <c r="D115" s="16">
-        <v>28</v>
-      </c>
+      <c r="A115" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="20"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="20"/>
       <c r="E115" s="29"/>
-      <c r="F115" s="23"/>
-      <c r="G115" s="23"/>
-      <c r="H115" s="23"/>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24">
+        <v>171</v>
+      </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B116" s="16"/>
       <c r="C116" s="16"/>
-      <c r="D116" s="16">
-        <v>34</v>
-      </c>
-      <c r="E116" s="29"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="28"/>
       <c r="F116" s="23"/>
-      <c r="G116" s="23"/>
+      <c r="G116" s="22">
+        <v>210</v>
+      </c>
       <c r="H116" s="23"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="33" t="s">
-        <v>121</v>
+      <c r="A117" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="B117" s="16"/>
       <c r="C117" s="16"/>
-      <c r="D117" s="18">
-        <v>45</v>
-      </c>
-      <c r="E117" s="29"/>
+      <c r="D117" s="16"/>
+      <c r="E117" s="28"/>
       <c r="F117" s="23"/>
-      <c r="G117" s="23"/>
+      <c r="G117" s="23">
+        <v>132</v>
+      </c>
       <c r="H117" s="23"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="B118" s="16"/>
       <c r="C118" s="16"/>
-      <c r="D118" s="16">
-        <v>30</v>
-      </c>
-      <c r="E118" s="29"/>
-      <c r="F118" s="23"/>
+      <c r="D118" s="16"/>
+      <c r="E118" s="28"/>
+      <c r="F118" s="22">
+        <v>154</v>
+      </c>
       <c r="G118" s="23"/>
       <c r="H118" s="23"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="B119" s="16"/>
       <c r="C119" s="16"/>
       <c r="D119" s="16"/>
-      <c r="E119" s="29"/>
+      <c r="E119" s="28"/>
       <c r="F119" s="23"/>
-      <c r="G119" s="22">
-        <v>254</v>
-      </c>
-      <c r="H119" s="23"/>
+      <c r="G119" s="23"/>
+      <c r="H119" s="23">
+        <v>179</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B120" s="16"/>
       <c r="C120" s="16"/>
       <c r="D120" s="16"/>
-      <c r="E120" s="29"/>
-      <c r="F120" s="23"/>
-      <c r="G120" s="22">
-        <v>264</v>
-      </c>
-      <c r="H120" s="23"/>
+      <c r="E120" s="28"/>
+      <c r="F120" s="23">
+        <v>97</v>
+      </c>
+      <c r="G120" s="23"/>
+      <c r="H120" s="23">
+        <v>192</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B121" s="16"/>
       <c r="C121" s="16"/>
       <c r="D121" s="16"/>
-      <c r="E121" s="29"/>
-      <c r="F121" s="23">
-        <v>99</v>
-      </c>
-      <c r="G121" s="23"/>
-      <c r="H121" s="23">
-        <v>218</v>
-      </c>
+      <c r="E121" s="28"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="22">
+        <v>204</v>
+      </c>
+      <c r="H121" s="23"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B122" s="16"/>
       <c r="C122" s="16"/>
       <c r="D122" s="16"/>
-      <c r="E122" s="29"/>
-      <c r="F122" s="22">
-        <v>160</v>
+      <c r="E122" s="28"/>
+      <c r="F122" s="23">
+        <v>116</v>
       </c>
       <c r="G122" s="23"/>
       <c r="H122" s="23"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B123" s="16"/>
       <c r="C123" s="16"/>
-      <c r="D123" s="16">
-        <v>26</v>
-      </c>
-      <c r="E123" s="29"/>
+      <c r="D123" s="16"/>
+      <c r="E123" s="28"/>
       <c r="F123" s="23"/>
-      <c r="G123" s="23"/>
+      <c r="G123" s="23">
+        <v>148</v>
+      </c>
       <c r="H123" s="23"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B124" s="20"/>
-      <c r="C124" s="20"/>
-      <c r="D124" s="20">
-        <v>31</v>
-      </c>
-      <c r="E124" s="30"/>
-      <c r="F124" s="24"/>
-      <c r="G124" s="24"/>
-      <c r="H124" s="24"/>
+      <c r="A124" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="23">
+        <v>200</v>
+      </c>
+      <c r="H124" s="23"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B125" s="16">
-        <v>249</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B125" s="16"/>
       <c r="C125" s="16"/>
       <c r="D125" s="16"/>
-      <c r="E125" s="29"/>
-      <c r="F125" s="22">
-        <v>187</v>
-      </c>
+      <c r="E125" s="28"/>
+      <c r="F125" s="23"/>
       <c r="G125" s="22">
-        <v>292</v>
-      </c>
-      <c r="H125" s="22">
-        <v>468</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="H125" s="23"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B126" s="16">
-        <v>206</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B126" s="16"/>
       <c r="C126" s="16"/>
       <c r="D126" s="16"/>
-      <c r="E126" s="29"/>
+      <c r="E126" s="28"/>
       <c r="F126" s="23"/>
-      <c r="G126" s="23"/>
+      <c r="G126" s="22">
+        <v>264</v>
+      </c>
       <c r="H126" s="23"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="15" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B127" s="16"/>
       <c r="C127" s="16"/>
       <c r="D127" s="16"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="22">
-        <v>172</v>
+      <c r="E127" s="28"/>
+      <c r="F127" s="23">
+        <v>99</v>
       </c>
       <c r="G127" s="23"/>
-      <c r="H127" s="22">
-        <v>298</v>
+      <c r="H127" s="23">
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="15" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="B128" s="16"/>
       <c r="C128" s="16"/>
       <c r="D128" s="16"/>
-      <c r="E128" s="29"/>
-      <c r="F128" s="23"/>
+      <c r="E128" s="28"/>
+      <c r="F128" s="22">
+        <v>160</v>
+      </c>
       <c r="G128" s="23"/>
-      <c r="H128" s="23">
-        <v>290</v>
-      </c>
+      <c r="H128" s="23"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B129" s="20"/>
-      <c r="C129" s="20"/>
-      <c r="D129" s="20"/>
-      <c r="E129" s="30"/>
-      <c r="F129" s="24"/>
-      <c r="G129" s="24"/>
-      <c r="H129" s="24">
-        <v>276</v>
+      <c r="A129" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B129" s="16"/>
+      <c r="C129" s="16"/>
+      <c r="D129" s="16"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="22">
+        <v>172</v>
+      </c>
+      <c r="G129" s="23"/>
+      <c r="H129" s="22">
+        <v>298</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="B130" s="16"/>
       <c r="C130" s="16"/>
       <c r="D130" s="16"/>
-      <c r="E130" s="29"/>
+      <c r="E130" s="28"/>
       <c r="F130" s="23"/>
-      <c r="G130" s="22">
-        <v>208</v>
-      </c>
-      <c r="H130" s="23"/>
+      <c r="G130" s="23"/>
+      <c r="H130" s="23">
+        <v>290</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B131" s="20">
-        <v>172</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B131" s="20"/>
       <c r="C131" s="20"/>
       <c r="D131" s="20"/>
-      <c r="E131" s="30"/>
+      <c r="E131" s="29"/>
       <c r="F131" s="24"/>
       <c r="G131" s="24"/>
-      <c r="H131" s="24"/>
+      <c r="H131" s="24">
+        <v>276</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="19" t="s">
+      <c r="A132" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B132" s="16"/>
+      <c r="C132" s="16"/>
+      <c r="D132" s="16"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="23"/>
+      <c r="G132" s="22">
+        <v>208</v>
+      </c>
+      <c r="H132" s="23"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B132" s="20"/>
-      <c r="C132" s="20"/>
-      <c r="D132" s="20"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="24"/>
-      <c r="G132" s="24"/>
-      <c r="H132" s="25">
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="30"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="25"/>
+      <c r="H133" s="38">
         <v>299</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B133" s="36">
-        <v>281</v>
-      </c>
-      <c r="C133" s="17"/>
-      <c r="D133" s="36">
-        <v>41</v>
-      </c>
-      <c r="E133" s="31"/>
-      <c r="F133" s="26"/>
-      <c r="G133" s="26">
-        <v>152</v>
-      </c>
-      <c r="H133" s="26">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H133" xr:uid="{575B943C-A161-443F-8BBF-F7A088F070C6}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H133">
-      <sortCondition descending="1" ref="C1:C133"/>
+      <sortCondition descending="1" ref="D1:D133"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>